<commit_message>
meerbeek data request, annual reports, harvest spreadsheet
</commit_message>
<xml_diff>
--- a/Meerbeek_Data_request.xlsx
+++ b/Meerbeek_Data_request.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20353"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Natural_Lakes_Research\Data\Federal_Aid_Projects\7027\Approach4\Approach4_Surveys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martysim\Documents\BMB-COC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D28F84-62D0-45C2-BEFB-ACD9F9975177}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{ACBF7B6C-0D46-4B0F-A99D-1DE3E0C0E58D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
   <si>
     <t>Lake</t>
   </si>
@@ -52,12 +51,42 @@
   </si>
   <si>
     <t>** CAP mean wt should only be from those fish captured during bimonthly EF samples from August to October (combined)</t>
+  </si>
+  <si>
+    <t>Blue</t>
+  </si>
+  <si>
+    <t>Center</t>
+  </si>
+  <si>
+    <t>North Twin</t>
+  </si>
+  <si>
+    <t>South Twin</t>
+  </si>
+  <si>
+    <t>Five Island</t>
+  </si>
+  <si>
+    <t>Silver</t>
+  </si>
+  <si>
+    <t>Storm</t>
+  </si>
+  <si>
+    <t>No fall standard runs in 2017</t>
+  </si>
+  <si>
+    <t>Calculated from each lake's spring l-w regression, applied to observed fall catch lengths (std runs), then averaged</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.0"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -67,12 +96,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -98,9 +133,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,16 +451,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2FD1FAC-C313-48A8-912D-419ABC40E4D1}">
-  <dimension ref="A1:G11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
@@ -455,14 +492,372 @@
         <v>6</v>
       </c>
     </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>2017</v>
+      </c>
+      <c r="E2">
+        <v>60835</v>
+      </c>
+      <c r="F2" s="2">
+        <v>448.3903345724907</v>
+      </c>
+      <c r="G2">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>2017</v>
+      </c>
+      <c r="E3">
+        <v>8675</v>
+      </c>
+      <c r="F3" s="2">
+        <v>263.32727272727271</v>
+      </c>
+      <c r="G3">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>2017</v>
+      </c>
+      <c r="E4">
+        <v>2057</v>
+      </c>
+      <c r="F4" s="2">
+        <v>19.869757174392937</v>
+      </c>
+      <c r="G4">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>2017</v>
+      </c>
+      <c r="E5">
+        <v>23204</v>
+      </c>
+      <c r="F5" s="2">
+        <v>68.644999999999996</v>
+      </c>
+      <c r="G5">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>2018</v>
+      </c>
+      <c r="C6">
+        <v>75.900000000000006</v>
+      </c>
+      <c r="E6">
+        <v>72140</v>
+      </c>
+      <c r="F6" s="2">
+        <v>543</v>
+      </c>
+      <c r="G6">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>2018</v>
+      </c>
+      <c r="C7">
+        <v>5.47</v>
+      </c>
+      <c r="E7">
+        <v>6466</v>
+      </c>
+      <c r="F7" s="2">
+        <v>194</v>
+      </c>
+      <c r="G7">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>2018</v>
+      </c>
+      <c r="C8">
+        <v>10.8</v>
+      </c>
+      <c r="E8">
+        <v>25798</v>
+      </c>
+      <c r="F8" s="2">
+        <v>187</v>
+      </c>
+      <c r="G8">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>2018</v>
+      </c>
+      <c r="C9">
+        <v>41.3</v>
+      </c>
+      <c r="E9">
+        <v>3816</v>
+      </c>
+      <c r="F9" s="2">
+        <v>34</v>
+      </c>
+      <c r="G9">
+        <v>453</v>
+      </c>
+    </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>12</v>
+      </c>
+      <c r="B10">
+        <v>2018</v>
+      </c>
+      <c r="C10">
+        <v>105</v>
+      </c>
+      <c r="E10">
+        <v>20661</v>
+      </c>
+      <c r="F10" s="2">
+        <v>62</v>
+      </c>
+      <c r="G10">
+        <v>600</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>2018</v>
+      </c>
+      <c r="C11">
+        <v>14.1</v>
+      </c>
+      <c r="E11">
+        <v>9755</v>
+      </c>
+      <c r="F11" s="2">
+        <v>96</v>
+      </c>
+      <c r="G11">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>2018</v>
+      </c>
+      <c r="C12">
+        <v>12.9</v>
+      </c>
+      <c r="E12">
+        <v>9251</v>
+      </c>
+      <c r="F12" s="2">
+        <v>11</v>
+      </c>
+      <c r="G12">
+        <v>3097</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>2019</v>
+      </c>
+      <c r="C13">
+        <v>191</v>
+      </c>
+      <c r="E13">
+        <v>25661</v>
+      </c>
+      <c r="F13" s="2">
+        <v>192</v>
+      </c>
+      <c r="G13">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>2019</v>
+      </c>
+      <c r="C14">
+        <v>6.1</v>
+      </c>
+      <c r="E14">
+        <v>1451</v>
+      </c>
+      <c r="F14" s="2">
+        <v>48</v>
+      </c>
+      <c r="G14">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>2019</v>
+      </c>
+      <c r="C15">
+        <v>9.81</v>
+      </c>
+      <c r="E15">
+        <v>19738</v>
+      </c>
+      <c r="F15" s="2">
+        <v>160.19999999999999</v>
+      </c>
+      <c r="G15">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16">
+        <v>2019</v>
+      </c>
+      <c r="C16">
+        <v>30.4</v>
+      </c>
+      <c r="E16">
+        <v>2487</v>
+      </c>
+      <c r="F16" s="2">
+        <v>34.5</v>
+      </c>
+      <c r="G16">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17">
+        <v>2019</v>
+      </c>
+      <c r="C17">
+        <v>195</v>
+      </c>
+      <c r="E17">
+        <v>14896</v>
+      </c>
+      <c r="F17" s="2">
+        <v>45.3</v>
+      </c>
+      <c r="G17">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18">
+        <v>2019</v>
+      </c>
+      <c r="C18">
+        <v>23.1</v>
+      </c>
+      <c r="E18">
+        <v>9174</v>
+      </c>
+      <c r="F18" s="2">
+        <v>93.8</v>
+      </c>
+      <c r="G18">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19">
+        <v>2019</v>
+      </c>
+      <c r="C19">
+        <v>20.3</v>
+      </c>
+      <c r="E19">
+        <v>15467</v>
+      </c>
+      <c r="F19" s="2">
+        <v>20.6</v>
+      </c>
+      <c r="G19">
+        <v>3097</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="3" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
entered meerbeek data to .xlsx sheet
</commit_message>
<xml_diff>
--- a/Meerbeek_Data_request.xlsx
+++ b/Meerbeek_Data_request.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
   <si>
     <t>Lake</t>
   </si>
@@ -35,9 +35,6 @@
     <t>CAP Catch/hr*</t>
   </si>
   <si>
-    <t>Mean Wt **</t>
-  </si>
-  <si>
     <t>MR Population Est</t>
   </si>
   <si>
@@ -78,14 +75,24 @@
   </si>
   <si>
     <t>Calculated from each lake's spring l-w regression, applied to observed fall catch lengths (std runs), then averaged</t>
+  </si>
+  <si>
+    <t>Mean Wt (grams)</t>
+  </si>
+  <si>
+    <t>Mean Wt ** ( pounds)</t>
+  </si>
+  <si>
+    <t>conversion grams to pounds</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="170" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -133,11 +140,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -463,13 +471,13 @@
     <col min="1" max="1" width="13.85546875" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" customWidth="1"/>
     <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="5.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -480,21 +488,27 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2">
         <v>2017</v>
@@ -509,9 +523,9 @@
         <v>269</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>2017</v>
@@ -526,9 +540,9 @@
         <v>220</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>2017</v>
@@ -543,9 +557,9 @@
         <v>453</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <v>2017</v>
@@ -560,9 +574,9 @@
         <v>600</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>2018</v>
@@ -570,6 +584,9 @@
       <c r="C6">
         <v>75.900000000000006</v>
       </c>
+      <c r="D6" s="4">
+        <v>3.0004938358701212</v>
+      </c>
       <c r="E6">
         <v>72140</v>
       </c>
@@ -579,10 +596,17 @@
       <c r="G6">
         <v>269</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <v>1361</v>
+      </c>
+      <c r="L6">
+        <f>J6/453.592</f>
+        <v>3.0004938358701212</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>2018</v>
@@ -590,6 +614,9 @@
       <c r="C7">
         <v>5.47</v>
       </c>
+      <c r="D7" s="4">
+        <v>4.6208927847051982</v>
+      </c>
       <c r="E7">
         <v>6466</v>
       </c>
@@ -599,10 +626,17 @@
       <c r="G7">
         <v>220</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <v>2096</v>
+      </c>
+      <c r="L7">
+        <f t="shared" ref="L7:L19" si="0">J7/453.592</f>
+        <v>4.6208927847051982</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B8">
         <v>2018</v>
@@ -610,6 +644,9 @@
       <c r="C8">
         <v>10.8</v>
       </c>
+      <c r="D8" s="4">
+        <v>6.2699518510026637</v>
+      </c>
       <c r="E8">
         <v>25798</v>
       </c>
@@ -619,10 +656,17 @@
       <c r="G8">
         <v>973</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <v>2844</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>6.2699518510026637</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9">
         <v>2018</v>
@@ -630,6 +674,9 @@
       <c r="C9">
         <v>41.3</v>
       </c>
+      <c r="D9" s="4">
+        <v>7.5420201414487034</v>
+      </c>
       <c r="E9">
         <v>3816</v>
       </c>
@@ -639,10 +686,17 @@
       <c r="G9">
         <v>453</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J9">
+        <v>3421</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>7.5420201414487034</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B10">
         <v>2018</v>
@@ -650,6 +704,9 @@
       <c r="C10">
         <v>105</v>
       </c>
+      <c r="D10" s="4">
+        <v>1.7570856628864706</v>
+      </c>
       <c r="E10">
         <v>20661</v>
       </c>
@@ -659,10 +716,17 @@
       <c r="G10">
         <v>600</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <v>797</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>1.7570856628864706</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>2018</v>
@@ -670,6 +734,9 @@
       <c r="C11">
         <v>14.1</v>
       </c>
+      <c r="D11" s="4">
+        <v>10.579992592461949</v>
+      </c>
       <c r="E11">
         <v>9755</v>
       </c>
@@ -679,10 +746,17 @@
       <c r="G11">
         <v>1041</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <v>4799</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>10.579992592461949</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12">
         <v>2018</v>
@@ -690,6 +764,9 @@
       <c r="C12">
         <v>12.9</v>
       </c>
+      <c r="D12" s="4">
+        <v>4.3188592391400205</v>
+      </c>
       <c r="E12">
         <v>9251</v>
       </c>
@@ -699,10 +776,17 @@
       <c r="G12">
         <v>3097</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <v>1959</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>4.3188592391400205</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B13">
         <v>2019</v>
@@ -710,6 +794,9 @@
       <c r="C13">
         <v>191</v>
       </c>
+      <c r="D13" s="4">
+        <v>2.8527839997178082</v>
+      </c>
       <c r="E13">
         <v>25661</v>
       </c>
@@ -719,10 +806,17 @@
       <c r="G13">
         <v>269</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J13">
+        <v>1294</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>2.8527839997178082</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B14">
         <v>2019</v>
@@ -730,6 +824,9 @@
       <c r="C14">
         <v>6.1</v>
       </c>
+      <c r="D14" s="4">
+        <v>5.0067020582373587</v>
+      </c>
       <c r="E14">
         <v>1451</v>
       </c>
@@ -739,10 +836,17 @@
       <c r="G14">
         <v>220</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <v>2271</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>5.0067020582373587</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15">
         <v>2019</v>
@@ -750,6 +854,9 @@
       <c r="C15">
         <v>9.81</v>
       </c>
+      <c r="D15" s="4">
+        <v>7.3502178168927141</v>
+      </c>
       <c r="E15">
         <v>19738</v>
       </c>
@@ -759,10 +866,17 @@
       <c r="G15">
         <v>973</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J15">
+        <v>3334</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>7.3502178168927141</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B16">
         <v>2019</v>
@@ -770,6 +884,9 @@
       <c r="C16">
         <v>30.4</v>
       </c>
+      <c r="D16" s="4">
+        <v>8.9088872819626452</v>
+      </c>
       <c r="E16">
         <v>2487</v>
       </c>
@@ -779,10 +896,17 @@
       <c r="G16">
         <v>453</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J16">
+        <v>4041</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>8.9088872819626452</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B17">
         <v>2019</v>
@@ -790,6 +914,9 @@
       <c r="C17">
         <v>195</v>
       </c>
+      <c r="D17" s="4">
+        <v>1.843066015273638</v>
+      </c>
       <c r="E17">
         <v>14896</v>
       </c>
@@ -799,10 +926,17 @@
       <c r="G17">
         <v>600</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J17">
+        <v>836</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="0"/>
+        <v>1.843066015273638</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B18">
         <v>2019</v>
@@ -810,6 +944,9 @@
       <c r="C18">
         <v>23.1</v>
       </c>
+      <c r="D18" s="4">
+        <v>11.214924425474877</v>
+      </c>
       <c r="E18">
         <v>9174</v>
       </c>
@@ -819,10 +956,17 @@
       <c r="G18">
         <v>1041</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J18">
+        <v>5087</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="0"/>
+        <v>11.214924425474877</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B19">
         <v>2019</v>
@@ -830,6 +974,9 @@
       <c r="C19">
         <v>20.3</v>
       </c>
+      <c r="D19" s="4">
+        <v>5.612973773787898</v>
+      </c>
       <c r="E19">
         <v>15467</v>
       </c>
@@ -839,25 +986,32 @@
       <c r="G19">
         <v>3097</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J19">
+        <v>2546</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="0"/>
+        <v>5.612973773787898</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B23" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="3" t="s">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="3" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="3" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
2020 annual report update
</commit_message>
<xml_diff>
--- a/Meerbeek_Data_request.xlsx
+++ b/Meerbeek_Data_request.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9648"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -463,21 +463,21 @@
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" customWidth="1"/>
     <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.44140625" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="26" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -506,7 +506,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -523,7 +523,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -540,7 +540,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -557,7 +557,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -574,7 +574,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -604,7 +604,7 @@
         <v>3.0004938358701212</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -634,7 +634,7 @@
         <v>4.6208927847051982</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -664,7 +664,7 @@
         <v>6.2699518510026637</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -694,7 +694,7 @@
         <v>7.5420201414487034</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -724,7 +724,7 @@
         <v>1.7570856628864706</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -754,7 +754,7 @@
         <v>10.579992592461949</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -784,7 +784,7 @@
         <v>4.3188592391400205</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -814,7 +814,7 @@
         <v>2.8527839997178082</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -822,7 +822,7 @@
         <v>2019</v>
       </c>
       <c r="C14">
-        <v>4.76</v>
+        <v>2.86</v>
       </c>
       <c r="D14" s="4">
         <v>5.0067020582373587</v>
@@ -844,7 +844,7 @@
         <v>5.0067020582373587</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -852,7 +852,7 @@
         <v>2019</v>
       </c>
       <c r="C15">
-        <v>9.2899999999999991</v>
+        <v>8.17</v>
       </c>
       <c r="D15" s="4">
         <v>7.3502178168927141</v>
@@ -874,7 +874,7 @@
         <v>7.3502178168927141</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -882,7 +882,7 @@
         <v>2019</v>
       </c>
       <c r="C16">
-        <v>6.1</v>
+        <v>5.33</v>
       </c>
       <c r="D16" s="4">
         <v>8.9088872819626452</v>
@@ -904,7 +904,7 @@
         <v>8.9088872819626452</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -912,7 +912,7 @@
         <v>2019</v>
       </c>
       <c r="C17">
-        <v>37.1</v>
+        <v>32.5</v>
       </c>
       <c r="D17" s="4">
         <v>1.843066015273638</v>
@@ -934,7 +934,7 @@
         <v>1.843066015273638</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -964,7 +964,7 @@
         <v>11.214924425474877</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -994,22 +994,22 @@
         <v>5.612973773787898</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B23" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B25" s="3" t="s">
         <v>16</v>
       </c>

</xml_diff>